<commit_message>
automating add products to cart from custom store
</commit_message>
<xml_diff>
--- a/DBSeedInfo.xlsx
+++ b/DBSeedInfo.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\p1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BBE43F-5A5E-484A-BABF-47F6D2AC2705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7D2300-771D-4551-860A-33D6E649F9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2805" yWindow="3600" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{2DDCEDC0-48E4-4BEF-B835-28279600D4F6}"/>
+    <workbookView xWindow="450" yWindow="3270" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{2DDCEDC0-48E4-4BEF-B835-28279600D4F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
     <sheet name="Vendors" sheetId="2" r:id="rId2"/>
-    <sheet name="Clients" sheetId="4" r:id="rId3"/>
+    <sheet name="ClientItems" sheetId="5" r:id="rId3"/>
+    <sheet name="Clients" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>Fjallraven - Foldsack No. 1 Backpack, Fits 15 Laptops</t>
   </si>
@@ -84,18 +85,12 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>Website</t>
   </si>
   <si>
     <t>Pega</t>
   </si>
   <si>
-    <t>http://localhost:3000</t>
-  </si>
-  <si>
     <t>https://training.openspan.com/</t>
   </si>
   <si>
@@ -196,6 +191,21 @@
   </si>
   <si>
     <t>Nathan''s Online Store</t>
+  </si>
+  <si>
+    <t>https://nathans-store.herokuapp.com/</t>
+  </si>
+  <si>
+    <t>Vendor Id</t>
+  </si>
+  <si>
+    <t>ClientId</t>
+  </si>
+  <si>
+    <t>ItemId</t>
+  </si>
+  <si>
+    <t>Quantity</t>
   </si>
 </sst>
 </file>
@@ -567,13 +577,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC8E10B-82B9-49AD-B014-3FACC33C2B8C}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="82.140625" customWidth="1"/>
+    <col min="1" max="1" width="95.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -582,7 +592,7 @@
         <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -590,7 +600,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>109.95</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -599,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>22.3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -608,7 +618,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>55.99</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -617,16 +627,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>15.99</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" s="1">
-        <v>695</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -635,7 +645,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>168</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -644,7 +654,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1">
-        <v>9.99</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -653,7 +663,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="1">
-        <v>10.99</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -662,7 +672,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="1">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -671,7 +681,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="1">
-        <v>109</v>
+        <v>2</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -680,7 +690,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>109</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -689,7 +699,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="1">
-        <v>114</v>
+        <v>2</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -698,7 +708,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="1">
-        <v>599</v>
+        <v>2</v>
       </c>
       <c r="C14" s="1"/>
     </row>
@@ -707,25 +717,25 @@
         <v>8</v>
       </c>
       <c r="B15" s="1">
-        <v>999.99</v>
+        <v>2</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1">
-        <v>56.99</v>
+        <v>2</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" s="1">
-        <v>29.95</v>
+        <v>2</v>
       </c>
       <c r="C17" s="1"/>
     </row>
@@ -734,25 +744,25 @@
         <v>7</v>
       </c>
       <c r="B18" s="1">
-        <v>39.99</v>
+        <v>2</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" s="1">
-        <v>9.85</v>
+        <v>2</v>
       </c>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1">
-        <v>7.95</v>
+        <v>2</v>
       </c>
       <c r="C20" s="1"/>
     </row>
@@ -761,202 +771,202 @@
         <v>6</v>
       </c>
       <c r="B21" s="1">
-        <v>12.99</v>
+        <v>2</v>
       </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1">
-        <v>263.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1">
-        <v>4.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1">
-        <v>46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1">
-        <v>7.76</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B35" s="1">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B36" s="1">
-        <v>21.36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1">
-        <v>15.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B38" s="1">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B39" s="1">
-        <v>19.46</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B40" s="1">
-        <v>21.06</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B41" s="1">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B42" s="1">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B43" s="1">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B44" s="1">
-        <v>28.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B45" s="1">
-        <v>43.9</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -969,14 +979,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{096D5FE7-5A7E-4E41-8C34-517D95946B47}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -984,23 +994,23 @@
         <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1012,11 +1022,202 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84088E9D-D6FD-42FB-B235-FA9915EAC8B7}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>42</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>18</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>27</v>
+      </c>
+      <c r="C16">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A114EF35-2A66-4FB1-9103-BAD7F96028A1}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,17 +1229,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
worked on a bunch of stuff
</commit_message>
<xml_diff>
--- a/DBSeedInfo.xlsx
+++ b/DBSeedInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\p1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7D2300-771D-4551-860A-33D6E649F9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBD2189-425F-41DE-B743-FC9F7EC57C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="3270" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{2DDCEDC0-48E4-4BEF-B835-28279600D4F6}"/>
+    <workbookView xWindow="4665" yWindow="3630" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{2DDCEDC0-48E4-4BEF-B835-28279600D4F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
   <si>
     <t>Fjallraven - Foldsack No. 1 Backpack, Fits 15 Laptops</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>nonExistant Item</t>
   </si>
 </sst>
 </file>
@@ -575,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC8E10B-82B9-49AD-B014-3FACC33C2B8C}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,6 +970,14 @@
       </c>
       <c r="B45" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B46" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1023,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84088E9D-D6FD-42FB-B235-FA9915EAC8B7}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="F16" sqref="F16:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1205,6 +1216,17 @@
       </c>
       <c r="C16">
         <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>45</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished automating pega addingtocart and checkout
</commit_message>
<xml_diff>
--- a/DBSeedInfo.xlsx
+++ b/DBSeedInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\p1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBD2189-425F-41DE-B743-FC9F7EC57C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B199B7D0-BCE8-4227-91C6-A8D41E88400C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4665" yWindow="3630" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{2DDCEDC0-48E4-4BEF-B835-28279600D4F6}"/>
   </bookViews>
@@ -1037,7 +1037,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:F17"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,7 +1204,7 @@
         <v>21</v>
       </c>
       <c r="C15">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>